<commit_message>
All 4 BPECs (OLC0637, 1512, 3094, 3095)
</commit_message>
<xml_diff>
--- a/Shigella_BPEC_competition/long_format_data/Growth_Curve_0-20h_Clean.xlsx
+++ b/Shigella_BPEC_competition/long_format_data/Growth_Curve_0-20h_Clean.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaolang/Dropbox/OLC-F-1915 Bacteriocin/Colicin Producer Genotypes Paper/Devon &amp; Ryan's thesis copy/Shigella BPEC competition - Devon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaolang/Dropbox/Github/Bacteriocin-OLC-F-1905/Shigella_BPEC_competition/Bacteriocin-OLC-F-1905/Shigella_BPEC_competition/long_format_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4010E404-5885-1E41-8D25-4FBE4747DC8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66617B99-541F-9347-8940-A00A8B09A371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="500" windowWidth="25420" windowHeight="14500" activeTab="1" xr2:uid="{BA92D02C-FF82-E045-9F07-BC5A1259C831}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="22">
   <si>
     <t>EC_ID</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Shg_EC_ratio</t>
+  </si>
+  <si>
+    <t>non-BPEC control</t>
   </si>
 </sst>
 </file>
@@ -3313,11 +3316,12 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -3349,7 +3353,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -3370,7 +3374,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3391,7 +3395,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -3412,7 +3416,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -3433,7 +3437,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -3454,7 +3458,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -3475,7 +3479,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -3496,7 +3500,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -3517,7 +3521,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>20</v>

</xml_diff>